<commit_message>
Adding 2 more offers for referrals, so we can ab test
Former-commit-id: a7e7f11ae851a88c30923c95bd239b3e5daa62fe
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_ReferralRewards.xlsx
+++ b/Docs/Content/HungryDragonContent_ReferralRewards.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="score" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -69,13 +69,37 @@
   </si>
   <si>
     <t>egg_epicGuaranteed</t>
+  </si>
+  <si>
+    <t>referralReward4</t>
+  </si>
+  <si>
+    <t>referralReward5</t>
+  </si>
+  <si>
+    <t>referralReward6</t>
+  </si>
+  <si>
+    <t>referralReward7</t>
+  </si>
+  <si>
+    <t>referralReward8</t>
+  </si>
+  <si>
+    <t>referralReward9</t>
+  </si>
+  <si>
+    <t>egg_babyGuaranteed</t>
+  </si>
+  <si>
+    <t>egg_rareGuaranteed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +137,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +182,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -232,11 +275,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -266,6 +322,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="scoreMultiplierDefinitions2" displayName="scoreMultiplierDefinitions2" ref="B4:G7" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="B4:G7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="scoreMultiplierDefinitions2" displayName="scoreMultiplierDefinitions2" ref="B4:G13" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B4:G13"/>
   <tableColumns count="6">
     <tableColumn id="1" name="{referralRewardsDefinitions}" dataDxfId="5"/>
     <tableColumn id="2" name="[sku]" dataDxfId="4"/>
@@ -800,10 +866,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:J7"/>
+  <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,16 +987,137 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="18">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="16">
+        <v>5</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="20">
+        <v>10</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="22">
+        <v>3</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="10">
+        <v>10</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="E5:G7"/>
+    <dataValidation allowBlank="1" sqref="E5:G13"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>